<commit_message>
component tracking xls update
</commit_message>
<xml_diff>
--- a/KiCad_PCB/Riscduino_Componets_Tracking.xlsx
+++ b/KiCad_PCB/Riscduino_Componets_Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vlsi\github\riscduino_board\KiCad_PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workarea\VLSI\github\riscduino_board\KiCad_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6344A9-2BE3-4828-A1AB-9774C781CB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF106B44-B323-4956-9CF8-9994D073C6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="420" windowWidth="27690" windowHeight="15060" xr2:uid="{3FCDD850-E4E8-4387-86E3-F9BFFF75D700}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3FCDD850-E4E8-4387-86E3-F9BFFF75D700}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Material!$A$3:$I$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -845,6 +846,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,27 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1199,8 +1200,8 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,12 +1222,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -1283,7 +1284,7 @@
       <c r="E4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="30" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1295,16 +1296,16 @@
       <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="34">
         <v>4.03</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="M4" s="34" t="s">
+      <c r="M4" s="35" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1325,7 +1326,7 @@
       <c r="E5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1335,10 +1336,10 @@
       <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="34"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
@@ -1357,14 +1358,14 @@
       <c r="E6" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="34"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
@@ -1383,7 +1384,7 @@
       <c r="E7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1393,10 +1394,10 @@
       <c r="I7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="35"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="34"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
@@ -1415,7 +1416,7 @@
       <c r="E8" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1425,10 +1426,10 @@
       <c r="I8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="34"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
@@ -1447,7 +1448,7 @@
       <c r="E9" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="30" t="s">
         <v>84</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1459,7 +1460,7 @@
       <c r="I9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="32" t="s">
         <v>139</v>
       </c>
       <c r="K9" s="36" t="s">
@@ -1468,7 +1469,7 @@
       <c r="L9" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="M9" s="35" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1489,7 +1490,7 @@
       <c r="E10" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1499,10 +1500,10 @@
       <c r="I10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="35"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
-      <c r="M10" s="34"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
@@ -1521,7 +1522,7 @@
       <c r="E11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="37"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1531,10 +1532,10 @@
       <c r="I11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="35"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
-      <c r="M11" s="34"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -1998,13 +1999,13 @@
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="38" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="37" t="s">
         <v>94</v>
       </c>
       <c r="F23" s="6">
@@ -2037,9 +2038,9 @@
         <v>195</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="31"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="30"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="6">
         <v>25</v>
       </c>
@@ -2147,20 +2148,20 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="32">
+      <c r="A27" s="39">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="38" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="37" t="s">
         <v>92</v>
       </c>
       <c r="F27" s="6">
@@ -2189,11 +2190,11 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="31"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="30"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="6">
         <v>25</v>
       </c>
@@ -3069,22 +3070,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="M4:M8"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="J4:J8"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="K4:K8"/>
-    <mergeCell ref="M4:M8"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C23:C24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M22" r:id="rId1" xr:uid="{7A47B26B-FB63-431B-AD45-421CCA2B1484}"/>

</xml_diff>